<commit_message>
System now cleans the milk inventory at the end of each day.
</commit_message>
<xml_diff>
--- a/TestResult-Day1.xlsx
+++ b/TestResult-Day1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Shop Name</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>Daily Sales</t>
-  </si>
-  <si>
-    <t>Ege</t>
   </si>
   <si>
     <t>Erdi</t>
@@ -183,22 +180,22 @@
         <v>18</v>
       </c>
       <c r="B3" t="n">
-        <v>25.0</v>
+        <v>47.25</v>
       </c>
       <c r="C3" t="n">
-        <v>50.0</v>
+        <v>20.0</v>
       </c>
       <c r="D3" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="E3" t="n">
-        <v>5.0</v>
+        <v>10.0</v>
       </c>
       <c r="F3" t="n">
-        <v>5.0</v>
+        <v>1.0</v>
       </c>
       <c r="G3" t="n">
-        <v>9.0</v>
+        <v>4.0</v>
       </c>
       <c r="H3" t="n">
         <v>10.0</v>
@@ -232,62 +229,6 @@
       </c>
       <c r="R3" t="n">
         <v>0.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="n">
-        <v>215.0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>12.0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1.62</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.059999999999999776</v>
-      </c>
-      <c r="F4" t="n">
-        <v>4.772</v>
-      </c>
-      <c r="G4" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>10.0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>130.0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>6.0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.9750000000000001</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0.44999999999999996</v>
-      </c>
-      <c r="N4" t="n">
-        <v>2.86375</v>
-      </c>
-      <c r="O4" t="n">
-        <v>3.6374999999999993</v>
-      </c>
-      <c r="P4" t="n">
-        <v>3.6374999999999993</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>3.6374999999999993</v>
-      </c>
-      <c r="R4" t="n">
-        <v>38.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>